<commit_message>
major code reformatting in capmin.py
</commit_message>
<xml_diff>
--- a/data/mnl/mnl.xlsx
+++ b/data/mnl/mnl.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="75" windowWidth="22515" windowHeight="9780" activeTab="5"/>
+    <workbookView xWindow="600" yWindow="75" windowWidth="22515" windowHeight="9780" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="6" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="80">
   <si>
     <t>Commodity</t>
   </si>
@@ -58,18 +58,12 @@
     <t>Direction</t>
   </si>
   <si>
-    <t>DH plant</t>
-  </si>
-  <si>
     <t>In</t>
   </si>
   <si>
     <t>Out</t>
   </si>
   <si>
-    <t>DC plant</t>
-  </si>
-  <si>
     <t>ratio</t>
   </si>
   <si>
@@ -77,9 +71,6 @@
   </si>
   <si>
     <t>cost-inv-var</t>
-  </si>
-  <si>
-    <t>Elec heating</t>
   </si>
   <si>
     <t>Storage</t>
@@ -210,13 +201,7 @@
     <t>other</t>
   </si>
   <si>
-    <t>demand</t>
-  </si>
-  <si>
     <t>Area</t>
-  </si>
-  <si>
-    <t>Power plant</t>
   </si>
   <si>
     <t>Non-spatial data (this file):</t>
@@ -275,9 +260,6 @@
     <t>Linear mixed-integer optimization model for urban energy infrastructure</t>
   </si>
   <si>
-    <t>cap-installed</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">area, type, nearest edge ID: is aggregated to </t>
     </r>
@@ -301,6 +283,63 @@
   </si>
   <si>
     <t>t rest</t>
+  </si>
+  <si>
+    <t>Elec heating domestic</t>
+  </si>
+  <si>
+    <t>District heating plant</t>
+  </si>
+  <si>
+    <t>District cooling plant</t>
+  </si>
+  <si>
+    <t>Gas power plant</t>
+  </si>
+  <si>
+    <t>Gas heating plant</t>
+  </si>
+  <si>
+    <t>Oil heating domestic</t>
+  </si>
+  <si>
+    <t>Elec heating plant</t>
+  </si>
+  <si>
+    <t>Gas heating domestic</t>
+  </si>
+  <si>
+    <t>Waste incineration plant</t>
+  </si>
+  <si>
+    <t>In Richter: GT (gas turbine), DT (steam turbine), so maybe split into two processes as well</t>
+  </si>
+  <si>
+    <t>In Richter: MV</t>
+  </si>
+  <si>
+    <t>In Richter: BK</t>
+  </si>
+  <si>
+    <t>In Richter: OA, ON</t>
+  </si>
+  <si>
+    <t>In Richter = Abbreviations as introduced for RES1 on page 72 in Richter2004</t>
+  </si>
+  <si>
+    <t>not mentioned</t>
+  </si>
+  <si>
+    <t>not mendioned</t>
+  </si>
+  <si>
+    <t>not mentioned (interesting)</t>
+  </si>
+  <si>
+    <t>Oil</t>
+  </si>
+  <si>
+    <t>Waste</t>
   </si>
 </sst>
 </file>
@@ -495,7 +534,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -524,8 +563,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -880,9 +917,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -904,7 +939,7 @@
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="17"/>
       <c r="C3" s="18" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="19"/>
@@ -917,7 +952,7 @@
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="17"/>
       <c r="C4" s="21" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
@@ -951,8 +986,8 @@
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="22"/>
-      <c r="C7" s="35" t="s">
-        <v>58</v>
+      <c r="C7" s="33" t="s">
+        <v>53</v>
       </c>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
@@ -964,12 +999,12 @@
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="22"/>
-      <c r="C8" s="32" t="s">
-        <v>36</v>
+      <c r="C8" s="30" t="s">
+        <v>33</v>
       </c>
       <c r="D8" s="13"/>
       <c r="E8" s="13" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
@@ -979,12 +1014,12 @@
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="22"/>
-      <c r="C9" s="32" t="s">
-        <v>37</v>
+      <c r="C9" s="30" t="s">
+        <v>34</v>
       </c>
       <c r="D9" s="13"/>
       <c r="E9" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
@@ -994,12 +1029,12 @@
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="22"/>
-      <c r="C10" s="33" t="s">
-        <v>38</v>
+      <c r="C10" s="31" t="s">
+        <v>35</v>
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="13" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
@@ -1009,12 +1044,12 @@
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="22"/>
-      <c r="C11" s="34" t="s">
-        <v>39</v>
+      <c r="C11" s="32" t="s">
+        <v>36</v>
       </c>
       <c r="D11" s="27"/>
       <c r="E11" s="27" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F11" s="27"/>
       <c r="G11" s="13"/>
@@ -1024,12 +1059,12 @@
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="22"/>
-      <c r="C12" s="32" t="s">
-        <v>40</v>
+      <c r="C12" s="30" t="s">
+        <v>37</v>
       </c>
       <c r="D12" s="13"/>
       <c r="E12" s="13" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
@@ -1039,12 +1074,12 @@
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="22"/>
-      <c r="C13" s="32" t="s">
-        <v>44</v>
+      <c r="C13" s="30" t="s">
+        <v>41</v>
       </c>
       <c r="D13" s="13"/>
       <c r="E13" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
@@ -1065,8 +1100,8 @@
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="22"/>
-      <c r="C15" s="35" t="s">
-        <v>59</v>
+      <c r="C15" s="33" t="s">
+        <v>54</v>
       </c>
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
@@ -1078,12 +1113,12 @@
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="22"/>
-      <c r="C16" s="32" t="s">
-        <v>41</v>
+      <c r="C16" s="30" t="s">
+        <v>38</v>
       </c>
       <c r="D16" s="13"/>
       <c r="E16" s="13" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
@@ -1093,12 +1128,12 @@
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="22"/>
-      <c r="C17" s="32" t="s">
-        <v>42</v>
+      <c r="C17" s="30" t="s">
+        <v>39</v>
       </c>
       <c r="D17" s="13"/>
       <c r="E17" s="13" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F17" s="13"/>
       <c r="G17" s="13"/>
@@ -1108,12 +1143,12 @@
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="22"/>
-      <c r="C18" s="32" t="s">
-        <v>43</v>
+      <c r="C18" s="30" t="s">
+        <v>40</v>
       </c>
       <c r="D18" s="13"/>
       <c r="E18" s="13" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
@@ -1256,7 +1291,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1276,22 +1311,22 @@
         <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1317,7 +1352,7 @@
         <v>0</v>
       </c>
       <c r="H2" s="3">
-        <v>250000</v>
+        <v>2500000</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1337,7 +1372,7 @@
         <v>0.6</v>
       </c>
       <c r="F3" s="11">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="G3" s="11">
         <v>0</v>
@@ -1405,27 +1440,27 @@
       <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="36" t="e">
+      <c r="C6" s="34" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="D6" s="36" t="e">
+      <c r="D6" s="34" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="E6" s="37" t="e">
+      <c r="E6" s="35" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="F6" s="38" t="e">
+      <c r="F6" s="36" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="G6" s="38" t="e">
+      <c r="G6" s="36" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="H6" s="36" t="e">
+      <c r="H6" s="34" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
@@ -1443,49 +1478,47 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" style="1" customWidth="1"/>
-    <col min="2" max="4" width="11.42578125" style="3"/>
-    <col min="5" max="5" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="3"/>
+    <col min="1" max="1" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="B2" s="3">
         <v>10000</v>
@@ -1497,18 +1530,18 @@
         <v>0</v>
       </c>
       <c r="E2" s="3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F2" s="3">
-        <v>100</v>
-      </c>
-      <c r="G2" s="3">
         <v>600</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="B3" s="3">
         <v>15000</v>
@@ -1520,18 +1553,18 @@
         <v>0</v>
       </c>
       <c r="E3" s="3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F3" s="3">
-        <v>100</v>
-      </c>
-      <c r="G3" s="3">
         <v>600</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="B4" s="3">
         <v>0</v>
@@ -1546,54 +1579,132 @@
         <v>0</v>
       </c>
       <c r="F4" s="3">
-        <v>0</v>
-      </c>
-      <c r="G4" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>800</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B5" s="3">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="3">
         <v>8000</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C6" s="3">
         <v>0.2</v>
       </c>
-      <c r="D5" s="3">
-        <v>0</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0</v>
-      </c>
-      <c r="F5" s="3">
-        <v>0</v>
-      </c>
-      <c r="G5" s="3">
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
         <v>400</v>
       </c>
+      <c r="H6" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="3">
+        <v>5000</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>99999</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>71</v>
+      </c>
     </row>
   </sheetData>
+  <dataValidations disablePrompts="1" count="5">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Fixed investment costs (€)" prompt="Up-front investment for building a plant, independent of size._x000a_Has value zero mainly for small-scale technologies." sqref="B1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Specific investment costs (€/kW)" prompt="Size-dependent part for building a plant." sqref="C1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Variable costs (€/kWh)" prompt="Operational costs to produce one unit of output, excluding fuel costs. Has value zero e.g. for PV or wind turbines (or if no sources are available)." sqref="D1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Minimum capacity (kW)" prompt="Smallest size a plant is typically available in. Has value zero for domestic technologies." sqref="E1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Maximum capacity (kW)" prompt="Biggest capacity a plant typically is available in." sqref="F1"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomRight" activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.42578125" style="1"/>
     <col min="4" max="4" width="11.42578125" style="9"/>
     <col min="5" max="16384" width="11.42578125" style="3"/>
   </cols>
@@ -1609,18 +1720,18 @@
         <v>11</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" s="9">
         <v>1</v>
@@ -1628,13 +1739,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" s="9">
         <v>0.3</v>
@@ -1642,27 +1753,27 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" s="9">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" s="9">
         <v>0.02</v>
@@ -1670,13 +1781,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="9">
         <v>1</v>
@@ -1684,13 +1795,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" s="9">
         <v>0.3</v>
@@ -1698,13 +1809,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" s="9">
         <v>0.7</v>
@@ -1712,13 +1823,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" s="9">
         <v>0.02</v>
@@ -1726,13 +1837,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" s="9">
         <v>1</v>
@@ -1740,27 +1851,27 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" s="9">
-        <v>1</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12" s="9">
         <v>1</v>
@@ -1768,13 +1879,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D13" s="9">
         <v>0.35</v>
@@ -1782,16 +1893,198 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D14" s="9">
         <v>0.02</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="9">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="9">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="9">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="9">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="9">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="9">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="9">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="9">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="9">
+        <v>0.55000000000000004</v>
       </c>
     </row>
   </sheetData>
@@ -1817,6 +2110,9 @@
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Input/output ratio (kWh/kWh)" prompt="Relative power flows in and out of processes. Sum of In and sum of Out should be equal to 1._x000a_For CO2, unit is kg/kWh." sqref="D1"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
@@ -1849,7 +2145,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1860,30 +2156,30 @@
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -1906,7 +2202,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -1929,7 +2225,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -1952,7 +2248,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>3</v>
@@ -1975,7 +2271,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>1</v>
@@ -2005,11 +2301,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2022,18 +2318,18 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B2" s="5">
         <v>0</v>
@@ -2044,7 +2340,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B3" s="5">
         <v>1</v>
@@ -2060,91 +2356,75 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F32" sqref="F32"/>
+      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="11.42578125" style="1"/>
-    <col min="3" max="3" width="11.42578125" style="31"/>
-    <col min="4" max="4" width="11.42578125" style="29"/>
-    <col min="5" max="16384" width="11.42578125" style="3"/>
+    <col min="3" max="3" width="11.42578125" style="29"/>
+    <col min="4" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="28" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1" s="28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="31">
+      <c r="C2" s="29">
         <v>0.03</v>
       </c>
-      <c r="D2" s="29">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="31">
+      <c r="C3" s="29">
         <v>0.03</v>
       </c>
-      <c r="D3" s="29">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="31">
+      <c r="C4" s="29">
         <v>0.03</v>
       </c>
-      <c r="D4" s="29">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="31">
+      <c r="C5" s="29">
         <v>0.03</v>
-      </c>
-      <c r="D5" s="29">
-        <v>2000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor changes in runmin.py and mnl dataset
</commit_message>
<xml_diff>
--- a/data/mnl/mnl.xlsx
+++ b/data/mnl/mnl.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="75" windowWidth="22515" windowHeight="9780" activeTab="3"/>
+    <workbookView xWindow="600" yWindow="75" windowWidth="22515" windowHeight="9780" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="6" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="77">
   <si>
     <t>Commodity</t>
   </si>
@@ -300,9 +300,6 @@
     <t>Gas heating plant</t>
   </si>
   <si>
-    <t>Oil heating domestic</t>
-  </si>
-  <si>
     <t>Elec heating plant</t>
   </si>
   <si>
@@ -321,25 +318,19 @@
     <t>In Richter: BK</t>
   </si>
   <si>
-    <t>In Richter: OA, ON</t>
-  </si>
-  <si>
-    <t>In Richter = Abbreviations as introduced for RES1 on page 72 in Richter2004</t>
-  </si>
-  <si>
     <t>not mentioned</t>
   </si>
   <si>
     <t>not mendioned</t>
   </si>
   <si>
-    <t>not mentioned (interesting)</t>
-  </si>
-  <si>
-    <t>Oil</t>
-  </si>
-  <si>
     <t>Waste</t>
+  </si>
+  <si>
+    <t>not mentioned (interesting: why?)</t>
+  </si>
+  <si>
+    <t>comment</t>
   </si>
 </sst>
 </file>
@@ -534,7 +525,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -584,6 +575,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1285,13 +1279,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1337,10 +1331,10 @@
         <v>6</v>
       </c>
       <c r="C2" s="3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D2" s="3">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="E2" s="7">
         <v>0.3</v>
@@ -1363,10 +1357,10 @@
         <v>6</v>
       </c>
       <c r="C3" s="3">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="D3" s="3">
-        <v>0</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="E3" s="7">
         <v>0.6</v>
@@ -1389,10 +1383,10 @@
         <v>6</v>
       </c>
       <c r="C4" s="3">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="D4" s="3">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="E4" s="7">
         <v>7.0000000000000007E-2</v>
@@ -1415,10 +1409,10 @@
         <v>6</v>
       </c>
       <c r="C5" s="3">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="D5" s="3">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="E5" s="7">
         <v>0.08</v>
@@ -1461,6 +1455,33 @@
         <v>#N/A</v>
       </c>
       <c r="H6" s="34" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="F7" s="11">
+        <v>0</v>
+      </c>
+      <c r="G7" s="11">
+        <v>0</v>
+      </c>
+      <c r="H7" s="34" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
@@ -1478,26 +1499,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8:A10"/>
+      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="11.42578125" style="3"/>
+    <col min="2" max="2" width="11.42578125" style="38"/>
+    <col min="3" max="4" width="11.42578125" style="3"/>
+    <col min="5" max="6" width="11.42578125" style="38"/>
+    <col min="7" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="37" t="s">
         <v>15</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -1506,21 +1530,21 @@
       <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>74</v>
+      <c r="H1" s="39" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="38">
         <v>10000</v>
       </c>
       <c r="C2" s="3">
@@ -1529,21 +1553,21 @@
       <c r="D2" s="3">
         <v>0</v>
       </c>
-      <c r="E2" s="3">
-        <v>100</v>
-      </c>
-      <c r="F2" s="3">
-        <v>600</v>
+      <c r="E2" s="38">
+        <v>100000</v>
+      </c>
+      <c r="F2" s="38">
+        <v>600000</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="38">
         <v>15000</v>
       </c>
       <c r="C3" s="3">
@@ -1552,44 +1576,44 @@
       <c r="D3" s="3">
         <v>0</v>
       </c>
-      <c r="E3" s="3">
-        <v>100</v>
-      </c>
-      <c r="F3" s="3">
-        <v>600</v>
+      <c r="E3" s="38">
+        <v>100000</v>
+      </c>
+      <c r="F3" s="38">
+        <v>600000</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="38">
         <v>0</v>
       </c>
       <c r="C4" s="3">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="D4" s="3">
         <v>0</v>
       </c>
-      <c r="E4" s="3">
-        <v>0</v>
-      </c>
-      <c r="F4" s="3">
+      <c r="E4" s="38">
+        <v>0</v>
+      </c>
+      <c r="F4" s="38">
         <v>800</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B5" s="3">
+        <v>66</v>
+      </c>
+      <c r="B5" s="38">
         <v>0</v>
       </c>
       <c r="C5" s="3">
@@ -1598,21 +1622,21 @@
       <c r="D5" s="3">
         <v>0</v>
       </c>
-      <c r="E5" s="3">
-        <v>0</v>
-      </c>
-      <c r="F5" s="3">
-        <v>0</v>
+      <c r="E5" s="38">
+        <v>50000</v>
+      </c>
+      <c r="F5" s="38">
+        <v>150000</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="38">
         <v>8000</v>
       </c>
       <c r="C6" s="3">
@@ -1621,21 +1645,21 @@
       <c r="D6" s="3">
         <v>0</v>
       </c>
-      <c r="E6" s="3">
-        <v>0</v>
-      </c>
-      <c r="F6" s="3">
-        <v>400</v>
+      <c r="E6" s="38">
+        <v>50000</v>
+      </c>
+      <c r="F6" s="38">
+        <v>400000</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="38">
         <v>5000</v>
       </c>
       <c r="C7" s="3">
@@ -1644,38 +1668,60 @@
       <c r="D7" s="3">
         <v>0</v>
       </c>
-      <c r="E7" s="3">
-        <v>0</v>
-      </c>
-      <c r="F7" s="3">
+      <c r="E7" s="38">
+        <v>0</v>
+      </c>
+      <c r="F7" s="38">
         <v>99999</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
+      </c>
+      <c r="B8" s="38">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3">
+        <v>2</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="38">
+        <v>0</v>
+      </c>
+      <c r="F8" s="38">
+        <v>0</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>68</v>
       </c>
+      <c r="B9" s="38">
+        <v>9000</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="38">
+        <v>0</v>
+      </c>
+      <c r="F9" s="38">
+        <v>0</v>
+      </c>
       <c r="H9" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1687,14 +1733,15 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Maximum capacity (kW)" prompt="Biggest capacity a plant typically is available in." sqref="F1"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1837,7 +1884,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>2</v>
@@ -1851,7 +1898,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>4</v>
@@ -1865,10 +1912,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>12</v>
@@ -1879,16 +1926,16 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="9">
-        <v>0.35</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1896,41 +1943,41 @@
         <v>64</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D14" s="9">
-        <v>0.02</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D15" s="9">
-        <v>1</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="9">
-        <v>0.98</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1938,83 +1985,83 @@
         <v>65</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D17" s="9">
-        <v>0.02</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D18" s="9">
-        <v>1</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D19" s="9">
-        <v>0.9</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D20" s="9">
-        <v>0.06</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D21" s="9">
-        <v>1</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="9">
-        <v>0.95</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -2022,68 +2069,54 @@
         <v>68</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>7</v>
+        <v>74</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D23" s="9">
-        <v>0.03</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>79</v>
+        <v>4</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D24" s="9">
-        <v>1</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D25" s="9">
-        <v>0.75</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D26" s="9">
-        <v>0.22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D27" s="9">
         <v>0.55000000000000004</v>
       </c>
     </row>
@@ -2301,11 +2334,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2356,13 +2389,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2396,18 +2429,18 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3" s="29">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -2418,13 +2451,57 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="29">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="29">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="29">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="29">
+      <c r="C8" s="29">
         <v>0.03</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="29">
+        <v>0.01</v>
       </c>
     </row>
   </sheetData>

</xml_diff>